<commit_message>
Started on grade reports.
</commit_message>
<xml_diff>
--- a/TestData/Schuljahre/SCHULJAHR_2016/Z_Halbjahr_1/Noten/Notentabelle_12.xlsx
+++ b/TestData/Schuljahre/SCHULJAHR_2016/Z_Halbjahr_1/Noten/Notentabelle_12.xlsx
@@ -736,7 +736,11 @@
         </is>
       </c>
       <c r="D9" s="4" t="n"/>
-      <c r="E9" s="7" t="n"/>
+      <c r="E9" s="7" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
       <c r="F9" s="7" t="inlineStr">
         <is>
           <t>2</t>
@@ -769,7 +773,7 @@
       </c>
       <c r="L9" s="7" t="inlineStr">
         <is>
-          <t>/</t>
+          <t>nt</t>
         </is>
       </c>
       <c r="M9" s="7" t="inlineStr">
@@ -807,7 +811,11 @@
           <t>2</t>
         </is>
       </c>
-      <c r="T9" s="7" t="n"/>
+      <c r="T9" s="7" t="inlineStr">
+        <is>
+          <t>2-</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="22.4" r="10">
       <c r="A10" s="3" t="inlineStr">
@@ -888,7 +896,7 @@
       </c>
       <c r="Q10" s="9" t="inlineStr">
         <is>
-          <t>/</t>
+          <t>nt</t>
         </is>
       </c>
       <c r="R10" s="9" t="inlineStr">
@@ -961,7 +969,7 @@
       </c>
       <c r="L11" s="9" t="inlineStr">
         <is>
-          <t>/</t>
+          <t>nt</t>
         </is>
       </c>
       <c r="M11" s="9" t="inlineStr">
@@ -976,7 +984,7 @@
       </c>
       <c r="O11" s="9" t="inlineStr">
         <is>
-          <t>/</t>
+          <t>nt</t>
         </is>
       </c>
       <c r="P11" s="9" t="inlineStr">
@@ -1001,7 +1009,7 @@
       </c>
       <c r="T11" s="9" t="inlineStr">
         <is>
-          <t>/</t>
+          <t>nt</t>
         </is>
       </c>
     </row>
@@ -1022,7 +1030,11 @@
         </is>
       </c>
       <c r="D12" s="4" t="n"/>
-      <c r="E12" s="7" t="n"/>
+      <c r="E12" s="7" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
       <c r="F12" s="7" t="inlineStr">
         <is>
           <t>4</t>
@@ -1055,7 +1067,7 @@
       </c>
       <c r="L12" s="7" t="inlineStr">
         <is>
-          <t>/</t>
+          <t>nt</t>
         </is>
       </c>
       <c r="M12" s="7" t="inlineStr">
@@ -1093,7 +1105,11 @@
           <t>3+</t>
         </is>
       </c>
-      <c r="T12" s="7" t="n"/>
+      <c r="T12" s="7" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="22.4" r="13">
       <c r="A13" s="3" t="inlineStr">
@@ -1174,7 +1190,7 @@
       </c>
       <c r="Q13" s="9" t="inlineStr">
         <is>
-          <t>/</t>
+          <t>nt</t>
         </is>
       </c>
       <c r="R13" s="9" t="inlineStr">
@@ -1210,7 +1226,11 @@
         </is>
       </c>
       <c r="D14" s="4" t="n"/>
-      <c r="E14" s="7" t="n"/>
+      <c r="E14" s="7" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
       <c r="F14" s="7" t="inlineStr">
         <is>
           <t>4-</t>
@@ -1281,7 +1301,11 @@
           <t>2-</t>
         </is>
       </c>
-      <c r="T14" s="7" t="n"/>
+      <c r="T14" s="7" t="inlineStr">
+        <is>
+          <t>3-</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="22.4" r="15">
       <c r="A15" s="3" t="inlineStr">
@@ -1312,57 +1336,57 @@
       </c>
       <c r="G15" s="9" t="inlineStr">
         <is>
+          <t>nt</t>
+        </is>
+      </c>
+      <c r="H15" s="9" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
+      <c r="I15" s="9" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
+      <c r="J15" s="9" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="K15" s="9" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="L15" s="8" t="inlineStr">
+        <is>
           <t>/</t>
         </is>
       </c>
-      <c r="H15" s="9" t="inlineStr">
+      <c r="M15" s="9" t="inlineStr">
         <is>
           <t>08</t>
         </is>
       </c>
-      <c r="I15" s="9" t="inlineStr">
+      <c r="N15" s="9" t="inlineStr">
         <is>
           <t>07</t>
         </is>
       </c>
-      <c r="J15" s="9" t="inlineStr">
+      <c r="O15" s="9" t="inlineStr">
         <is>
           <t>11</t>
         </is>
       </c>
-      <c r="K15" s="9" t="inlineStr">
+      <c r="P15" s="9" t="inlineStr">
         <is>
           <t>02</t>
         </is>
       </c>
-      <c r="L15" s="8" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="M15" s="9" t="inlineStr">
-        <is>
-          <t>08</t>
-        </is>
-      </c>
-      <c r="N15" s="9" t="inlineStr">
-        <is>
-          <t>07</t>
-        </is>
-      </c>
-      <c r="O15" s="9" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="P15" s="9" t="inlineStr">
-        <is>
-          <t>02</t>
-        </is>
-      </c>
       <c r="Q15" s="9" t="inlineStr">
         <is>
-          <t>/</t>
+          <t>nt</t>
         </is>
       </c>
       <c r="R15" s="9" t="inlineStr">
@@ -1403,33 +1427,81 @@
           <t>/</t>
         </is>
       </c>
-      <c r="F16" s="9" t="n"/>
+      <c r="F16" s="9" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
       <c r="G16" s="9" t="inlineStr">
         <is>
+          <t>nt</t>
+        </is>
+      </c>
+      <c r="H16" s="9" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
+      <c r="I16" s="9" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
+      <c r="J16" s="9" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="K16" s="9" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="L16" s="8" t="inlineStr">
+        <is>
           <t>/</t>
         </is>
       </c>
-      <c r="H16" s="9" t="n"/>
-      <c r="I16" s="9" t="n"/>
-      <c r="J16" s="9" t="n"/>
-      <c r="K16" s="9" t="n"/>
-      <c r="L16" s="8" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="M16" s="9" t="n"/>
-      <c r="N16" s="9" t="n"/>
-      <c r="O16" s="9" t="n"/>
-      <c r="P16" s="9" t="n"/>
+      <c r="M16" s="9" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
+      <c r="N16" s="9" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
+      </c>
+      <c r="O16" s="9" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="P16" s="9" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
       <c r="Q16" s="9" t="inlineStr">
         <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="R16" s="9" t="n"/>
-      <c r="S16" s="9" t="n"/>
-      <c r="T16" s="9" t="n"/>
+          <t>nt</t>
+        </is>
+      </c>
+      <c r="R16" s="9" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
+      <c r="S16" s="9" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="T16" s="9" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <sheetProtection autoFilter="1" deleteColumns="1" deleteRows="1" formatCells="1" formatColumns="1" formatRows="1" insertColumns="1" insertHyperlinks="1" insertRows="1" objects="0" pivotTables="1" scenarios="0" selectLockedCells="0" selectUnlockedCells="0" sheet="1" sort="1"/>
@@ -1439,9 +1511,12 @@
     <mergeCell ref="C3:S3"/>
     <mergeCell ref="C4:S4"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="E9 F9 G9 H9 I9 J9 L9 M9 N9 O9 P9 Q9 R9 S9 T9 F10 H10 I10 J10 K10 L10 M10 N10 O10 P10 Q10 R10 S10 T10 F11 G11 H11 I11 J11 K11 L11 M11 N11 O11 P11 Q11 R11 S11 T11 E12 F12 G12 H12 I12 J12 L12 M12 N12 O12 P12 Q12 R12 S12 T12 F13 G13 H13 I13 J13 K13 L13 M13 N13 O13 P13 Q13 R13 S13 T13 E14 F14 G14 H14 I14 J14 L14 M14 N14 O14 P14 Q14 R14 S14 T14 F15 G15 H15 I15 J15 K15 M15 N15 O15 P15 Q15 R15 S15 T15 F16 G16 H16 I16 J16 K16 M16 N16 O16 P16 Q16 R16 S16 T16" type="list">
+  <dataValidations count="2">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="E9 F9 G9 H9 I9 J9 L9 M9 N9 O9 P9 Q9 R9 S9 T9 E12 F12 G12 H12 I12 J12 L12 M12 N12 O12 P12 Q12 R12 S12 T12 E14 F14 G14 H14 I14 J14 L14 M14 N14 O14 P14 Q14 R14 S14 T14" type="list">
       <formula1>"1+,1,1-,2+,2,2-,3+,3,3-,4+,4,4-,5+,5,5-,6,nb,nt,t,*"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="F10 H10 I10 J10 K10 L10 M10 N10 O10 P10 Q10 R10 S10 T10 F11 G11 H11 I11 J11 K11 L11 M11 N11 O11 P11 Q11 R11 S11 T11 F13 G13 H13 I13 J13 K13 L13 M13 N13 O13 P13 Q13 R13 S13 T13 F15 G15 H15 I15 J15 K15 M15 N15 O15 P15 Q15 R15 S15 T15 F16 G16 H16 I16 J16 K16 M16 N16 O16 P16 Q16 R16 S16 T16" type="list">
+      <formula1>"15,14,13,12,11,10,09,08,07,06,05,04,03,02,01,00,nb,nt,t,*"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>